<commit_message>
Update to list - only pregnancies
</commit_message>
<xml_diff>
--- a/app/config/tables/PREGNANCIES/Forms/PREGNANCYFU/PREGNANCYFU.xlsx
+++ b/app/config/tables/PREGNANCIES/Forms/PREGNANCYFU/PREGNANCYFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E16048D-74D1-4DB0-94BA-32144D000E8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EE0922-6765-44A5-9C3E-92253F6505CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1206,7 +1206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
@@ -3177,9 +3177,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3476,6 +3476,9 @@
       <c r="D28" s="13"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:G19">
+    <sortCondition ref="G3:G19"/>
+  </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Error in NVNMAB constraints
</commit_message>
<xml_diff>
--- a/app/config/tables/PREGNANCIES/Forms/PREGNANCYFU/PREGNANCYFU.xlsx
+++ b/app/config/tables/PREGNANCIES/Forms/PREGNANCYFU/PREGNANCYFU.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5796EA15-BFD3-4E9C-A426-EC57FDAEF689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D782824-6E0B-4B67-A32C-4EEBC282C8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,12 +510,6 @@
     <t>Local de nascimento</t>
   </si>
   <si>
-    <t>data("GEM") != null || data("ESTADOGRAV") != 1 || data("NVNNAM") == 3</t>
-  </si>
-  <si>
-    <t>data("LOCPAR") != null || data("ESTADOGRAV") != 1 || data("NVNNAM") == 3</t>
-  </si>
-  <si>
     <t>PARTAB</t>
   </si>
   <si>
@@ -912,6 +906,12 @@
   </si>
   <si>
     <t>Has scar, uncertain if BCG</t>
+  </si>
+  <si>
+    <t>data("LOCPAR") != null || data("ESTADOGRAV") != 1 || data("NVNMAB") == 3</t>
+  </si>
+  <si>
+    <t>data("GEM") != null || data("ESTADOGRAV") != 1 || data("NVNMAB") == 3</t>
   </si>
 </sst>
 </file>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1461,8 +1461,8 @@
   <dimension ref="A1:T102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,13 +1542,13 @@
         <v>44</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1590,10 +1590,10 @@
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="S5" s="12" t="b">
         <v>1</v>
@@ -1604,10 +1604,10 @@
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S6" s="12" t="b">
         <v>1</v>
@@ -1618,10 +1618,10 @@
         <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="S7" s="12" t="b">
         <v>1</v>
@@ -1663,7 +1663,7 @@
         <v>60</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G10" t="s">
         <v>121</v>
@@ -1680,28 +1680,28 @@
         <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
       </c>
       <c r="K11" t="s">
+        <v>244</v>
+      </c>
+      <c r="L11" t="s">
+        <v>245</v>
+      </c>
+      <c r="M11" t="s">
         <v>246</v>
       </c>
-      <c r="L11" t="s">
-        <v>247</v>
-      </c>
-      <c r="M11" t="s">
-        <v>248</v>
-      </c>
       <c r="Q11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1720,10 +1720,10 @@
         <v>35</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S14" s="12" t="b">
         <v>1</v>
@@ -1770,10 +1770,10 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S18" s="12" t="b">
         <v>1</v>
@@ -1814,7 +1814,7 @@
         <v>28</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G21" s="22" t="s">
         <v>112</v>
@@ -1823,13 +1823,13 @@
         <v>111</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P21" s="12" t="b">
         <v>0</v>
@@ -1852,7 +1852,7 @@
         <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="2:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1866,10 +1866,10 @@
         <v>35</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S26" s="12" t="b">
         <v>1</v>
@@ -1880,10 +1880,10 @@
         <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G27" t="s">
         <v>100</v>
@@ -1892,16 +1892,16 @@
         <v>101</v>
       </c>
       <c r="K27" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L27" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="M27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1937,10 +1937,10 @@
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S32" s="12" t="b">
         <v>1</v>
@@ -1953,10 +1953,10 @@
         <v>35</v>
       </c>
       <c r="G33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="S33" s="12" t="b">
         <v>1</v>
@@ -1969,10 +1969,10 @@
         <v>35</v>
       </c>
       <c r="G34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="S34" s="12" t="b">
         <v>1</v>
@@ -1985,10 +1985,10 @@
         <v>35</v>
       </c>
       <c r="G35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="S35" s="12" t="b">
         <v>1</v>
@@ -2001,10 +2001,10 @@
         <v>35</v>
       </c>
       <c r="G36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H36" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="S36" s="12" t="b">
         <v>1</v>
@@ -2017,10 +2017,10 @@
         <v>35</v>
       </c>
       <c r="G37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="S37" s="12" t="b">
         <v>1</v>
@@ -2033,10 +2033,10 @@
         <v>35</v>
       </c>
       <c r="G38" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H38" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S38" s="12" t="b">
         <v>1</v>
@@ -2049,10 +2049,10 @@
         <v>35</v>
       </c>
       <c r="G39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H39" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="S39" s="12" t="b">
         <v>1</v>
@@ -2063,25 +2063,25 @@
         <v>51</v>
       </c>
       <c r="E40" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F40" t="s">
         <v>50</v>
       </c>
       <c r="G40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K40" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L40" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="M40" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2099,7 +2099,7 @@
         <v>67</v>
       </c>
       <c r="C43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2115,10 +2115,10 @@
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
       <c r="G45" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S45" s="12" t="b">
         <v>1</v>
@@ -2141,7 +2141,7 @@
         <v>88</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2167,10 +2167,10 @@
         <v>35</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S50" s="12" t="b">
         <v>1</v>
@@ -2196,10 +2196,10 @@
         <v>139</v>
       </c>
       <c r="L51" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M51" s="25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
@@ -2225,10 +2225,10 @@
         <v>35</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S55" s="12" t="b">
         <v>1</v>
@@ -2251,7 +2251,7 @@
         <v>157</v>
       </c>
       <c r="K56" t="s">
-        <v>159</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
@@ -2259,7 +2259,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.25">
@@ -2270,16 +2270,16 @@
         <v>53</v>
       </c>
       <c r="F58" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G58" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="G58" s="17" t="s">
-        <v>162</v>
-      </c>
       <c r="H58" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K58" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.25">
@@ -2292,7 +2292,7 @@
         <v>67</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
@@ -2303,28 +2303,28 @@
         <v>53</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G61" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K61" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D62" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I62" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
         <v>67</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.25">
@@ -2355,10 +2355,10 @@
         <v>35</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S67" s="12" t="b">
         <v>1</v>
@@ -2366,30 +2366,30 @@
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
+        <v>254</v>
+      </c>
+      <c r="E68" t="s">
+        <v>255</v>
+      </c>
+      <c r="F68" t="s">
         <v>256</v>
       </c>
-      <c r="E68" t="s">
-        <v>257</v>
-      </c>
-      <c r="F68" t="s">
-        <v>258</v>
-      </c>
       <c r="G68" s="17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E69" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F69" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G69" s="17" t="s">
         <v>156</v>
@@ -2398,21 +2398,21 @@
         <v>157</v>
       </c>
       <c r="K69" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T69" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
+        <v>258</v>
+      </c>
+      <c r="E70" t="s">
         <v>260</v>
       </c>
-      <c r="E70" t="s">
-        <v>262</v>
-      </c>
       <c r="F70" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="S70" s="13" t="b">
         <v>1</v>
@@ -2423,7 +2423,7 @@
         <v>67</v>
       </c>
       <c r="C71" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D71"/>
       <c r="E71"/>
@@ -2437,7 +2437,7 @@
         <v>67</v>
       </c>
       <c r="C72" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D72"/>
       <c r="E72"/>
@@ -2453,16 +2453,16 @@
         <v>60</v>
       </c>
       <c r="F73" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G73" t="s">
+        <v>280</v>
+      </c>
+      <c r="H73" t="s">
+        <v>281</v>
+      </c>
+      <c r="K73" s="13" t="s">
         <v>282</v>
-      </c>
-      <c r="H73" t="s">
-        <v>283</v>
-      </c>
-      <c r="K73" s="13" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.25">
@@ -2476,16 +2476,16 @@
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C75"/>
       <c r="D75" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E75"/>
       <c r="F75" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G75"/>
       <c r="H75"/>
       <c r="I75" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="S75" s="13" t="b">
         <v>1</v>
@@ -2517,10 +2517,10 @@
         <v>35</v>
       </c>
       <c r="G80" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S80" s="12" t="b">
         <v>1</v>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="J81" s="13"/>
       <c r="K81" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" spans="2:19" x14ac:dyDescent="0.25">
@@ -2562,7 +2562,7 @@
         <v>67</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="2:19" x14ac:dyDescent="0.25">
@@ -2575,10 +2575,10 @@
         <v>35</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S86" s="12" t="b">
         <v>1</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="91" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="92" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2634,10 +2634,10 @@
         <v>35</v>
       </c>
       <c r="G93" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="94" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2645,10 +2645,10 @@
         <v>35</v>
       </c>
       <c r="G94" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H94" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="95" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2671,10 +2671,10 @@
         <v>35</v>
       </c>
       <c r="G98" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S98" s="12" t="b">
         <v>1</v>
@@ -2713,13 +2713,13 @@
         <v>60</v>
       </c>
       <c r="F101" t="s">
+        <v>208</v>
+      </c>
+      <c r="G101" t="s">
+        <v>209</v>
+      </c>
+      <c r="H101" t="s">
         <v>210</v>
-      </c>
-      <c r="G101" t="s">
-        <v>211</v>
-      </c>
-      <c r="H101" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="102" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2898,7 +2898,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B12" t="str">
         <f>"1"</f>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B13" t="str">
         <f>"2"</f>
@@ -2928,22 +2928,22 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B14" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B15" t="str">
         <f>"33"</f>
@@ -2964,7 +2964,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B17" s="13" t="str">
         <f>"1"</f>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B18" s="13" t="str">
         <f>"2"</f>
@@ -3007,10 +3007,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3055,7 +3055,7 @@
         <v>91</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3169,10 +3169,10 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D32" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -3213,22 +3213,22 @@
     </row>
     <row r="36" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B36" t="str">
         <f>"8888"</f>
         <v>8888</v>
       </c>
       <c r="C36" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D36" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B37" t="str">
         <f>"9999"</f>
@@ -3908,41 +3908,41 @@
         <v>134</v>
       </c>
       <c r="I1" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>275</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
+        <v>269</v>
+      </c>
+      <c r="J2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="J2" t="s">
-        <v>272</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J3" t="s">
+        <v>270</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -3969,13 +3969,13 @@
         <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H5" s="24" t="s">
         <v>135</v>
@@ -4120,7 +4120,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4180,7 +4180,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
@@ -4191,7 +4191,7 @@
     </row>
     <row r="9" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
@@ -4202,7 +4202,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -4213,7 +4213,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
@@ -4222,7 +4222,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4249,7 +4249,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B15" t="s">
         <v>51</v>
@@ -4260,7 +4260,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B17" t="s">
         <v>60</v>
@@ -4315,7 +4315,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s">
         <v>51</v>
@@ -4326,7 +4326,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
@@ -4337,7 +4337,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
@@ -4348,7 +4348,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
@@ -4359,7 +4359,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -4381,7 +4381,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B27" t="s">
         <v>51</v>
@@ -4392,7 +4392,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B28" t="s">
         <v>60</v>
@@ -4403,7 +4403,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
@@ -4412,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4450,7 +4450,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
         <v>51</v>
@@ -4461,7 +4461,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
         <v>51</v>
@@ -4472,10 +4472,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B36" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C36" t="b">
         <v>1</v>
@@ -4483,10 +4483,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B37" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -4494,10 +4494,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B38" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C38" t="b">
         <v>1</v>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B39" t="s">
         <v>60</v>
@@ -4528,7 +4528,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B41" t="s">
         <v>48</v>
@@ -4539,7 +4539,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B42" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Option if woman still in HC/hospital
</commit_message>
<xml_diff>
--- a/app/config/tables/PREGNANCIES/Forms/PREGNANCYFU/PREGNANCYFU.xlsx
+++ b/app/config/tables/PREGNANCIES/Forms/PREGNANCYFU/PREGNANCYFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D782824-6E0B-4B67-A32C-4EEBC282C8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0ADDDC-B9CF-49E7-8C70-A5DE099F8CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="292">
   <si>
     <t>setting_name</t>
   </si>
@@ -912,6 +912,15 @@
   </si>
   <si>
     <t>data("GEM") != null || data("ESTADOGRAV") != 1 || data("NVNMAB") == 3</t>
+  </si>
+  <si>
+    <t>PlaceOfBirthReturn</t>
+  </si>
+  <si>
+    <t>Woman is still at the centre/hospital</t>
+  </si>
+  <si>
+    <t>Mulher ainda está no centro/hospital</t>
   </si>
 </sst>
 </file>
@@ -1460,9 +1469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:T102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,7 +2309,7 @@
         <v>51</v>
       </c>
       <c r="E61" t="s">
-        <v>53</v>
+        <v>289</v>
       </c>
       <c r="F61" s="13" t="s">
         <v>159</v>
@@ -2735,16 +2744,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="3" bestFit="1" customWidth="1"/>
@@ -3213,82 +3222,118 @@
     </row>
     <row r="36" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>289</v>
+      </c>
+      <c r="B36" s="13" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>289</v>
+      </c>
+      <c r="B37" s="13" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>289</v>
+      </c>
+      <c r="B38" s="10" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>289</v>
+      </c>
+      <c r="B39" s="13" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>260</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B41" t="str">
         <f>"8888"</f>
         <v>8888</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C41" t="s">
         <v>261</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D41" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="42" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>260</v>
       </c>
-      <c r="B37" t="str">
+      <c r="B42" t="str">
         <f>"9999"</f>
         <v>9999</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C42" t="s">
         <v>56</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D42" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="18"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="F40" s="13"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
-      <c r="B43" s="12"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
-      <c r="B44" s="12"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
+      <c r="D44" s="18"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
-      <c r="B45" s="12"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
+      <c r="F45" s="13"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
@@ -3298,69 +3343,69 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-    </row>
-    <row r="48" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="12"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-    </row>
-    <row r="49" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="12"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-    </row>
-    <row r="50" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="12"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="12"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-    </row>
-    <row r="51" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-    </row>
-    <row r="52" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="13"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+    </row>
+    <row r="54" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+    </row>
+    <row r="55" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+    </row>
+    <row r="57" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
@@ -3381,52 +3426,52 @@
       <c r="D60" s="14"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
+      <c r="A61" s="14"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="19"/>
+      <c r="B62" s="13"/>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
-      <c r="B63" s="19"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
@@ -3532,62 +3577,62 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
-      <c r="B86" s="19"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="13"/>
-      <c r="B87" s="19"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
-      <c r="B88" s="19"/>
+      <c r="B88" s="20"/>
       <c r="C88" s="21"/>
       <c r="D88" s="21"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
-      <c r="B89" s="19"/>
+      <c r="B89" s="20"/>
       <c r="C89" s="21"/>
-      <c r="D89" s="14"/>
+      <c r="D89" s="21"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
-      <c r="B90" s="19"/>
+      <c r="B90" s="20"/>
       <c r="C90" s="21"/>
-      <c r="D90" s="14"/>
+      <c r="D90" s="21"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" s="19"/>
-      <c r="C91" s="15"/>
+      <c r="C91" s="14"/>
       <c r="D91" s="14"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
       <c r="B92" s="19"/>
-      <c r="C92" s="15"/>
+      <c r="C92" s="14"/>
       <c r="D92" s="14"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
       <c r="B93" s="19"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94" s="19"/>
-      <c r="C94" s="15"/>
+      <c r="C94" s="21"/>
       <c r="D94" s="14"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="13"/>
       <c r="B95" s="19"/>
-      <c r="C95" s="15"/>
+      <c r="C95" s="21"/>
       <c r="D95" s="14"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3605,7 +3650,7 @@
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
       <c r="B98" s="19"/>
-      <c r="C98" s="15"/>
+      <c r="C98" s="14"/>
       <c r="D98" s="14"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3616,25 +3661,25 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
-      <c r="B100" s="13"/>
+      <c r="B100" s="19"/>
       <c r="C100" s="15"/>
       <c r="D100" s="14"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
-      <c r="B101" s="13"/>
+      <c r="B101" s="19"/>
       <c r="C101" s="15"/>
       <c r="D101" s="14"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
-      <c r="B102" s="13"/>
+      <c r="B102" s="19"/>
       <c r="C102" s="15"/>
       <c r="D102" s="14"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
-      <c r="B103" s="13"/>
+      <c r="B103" s="19"/>
       <c r="C103" s="15"/>
       <c r="D103" s="14"/>
     </row>
@@ -3646,7 +3691,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="13"/>
-      <c r="B105" s="19"/>
+      <c r="B105" s="13"/>
       <c r="C105" s="15"/>
       <c r="D105" s="14"/>
     </row>
@@ -3664,19 +3709,19 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="13"/>
-      <c r="B108" s="19"/>
+      <c r="B108" s="13"/>
       <c r="C108" s="15"/>
       <c r="D108" s="14"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
-      <c r="B109" s="13"/>
+      <c r="B109" s="19"/>
       <c r="C109" s="15"/>
       <c r="D109" s="14"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="13"/>
-      <c r="B110" s="13"/>
+      <c r="B110" s="19"/>
       <c r="C110" s="15"/>
       <c r="D110" s="14"/>
     </row>
@@ -3688,13 +3733,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
-      <c r="B112" s="19"/>
+      <c r="B112" s="13"/>
       <c r="C112" s="15"/>
       <c r="D112" s="14"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
-      <c r="B113" s="13"/>
+      <c r="B113" s="19"/>
       <c r="C113" s="15"/>
       <c r="D113" s="14"/>
     </row>
@@ -3707,18 +3752,18 @@
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
-      <c r="C115" s="14"/>
+      <c r="C115" s="15"/>
       <c r="D115" s="14"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
-      <c r="B116" s="19"/>
+      <c r="B116" s="13"/>
       <c r="C116" s="15"/>
       <c r="D116" s="14"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
-      <c r="B117" s="13"/>
+      <c r="B117" s="19"/>
       <c r="C117" s="15"/>
       <c r="D117" s="14"/>
     </row>
@@ -3737,7 +3782,7 @@
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
       <c r="B120" s="13"/>
-      <c r="C120" s="15"/>
+      <c r="C120" s="14"/>
       <c r="D120" s="14"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3761,96 +3806,126 @@
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
-      <c r="C124" s="14"/>
+      <c r="C124" s="15"/>
       <c r="D124" s="14"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
-      <c r="C125" s="14"/>
+      <c r="C125" s="15"/>
       <c r="D125" s="14"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
       <c r="B126" s="19"/>
-      <c r="C126" s="14"/>
+      <c r="C126" s="15"/>
       <c r="D126" s="14"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="7"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="15"/>
+      <c r="D127" s="14"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="7"/>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="7"/>
-      <c r="C129"/>
-      <c r="D129"/>
-    </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="7"/>
-      <c r="C130"/>
-      <c r="D130"/>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="7"/>
-      <c r="C131"/>
-      <c r="D131"/>
-    </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="15"/>
+      <c r="D128" s="14"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="13"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="13"/>
+      <c r="B130" s="13"/>
+      <c r="C130" s="14"/>
+      <c r="D130" s="14"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="13"/>
+      <c r="B131" s="19"/>
+      <c r="C131" s="14"/>
+      <c r="D131" s="14"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="7"/>
-      <c r="C132"/>
-      <c r="D132"/>
-    </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="7"/>
-      <c r="C133"/>
-      <c r="D133"/>
-    </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="7"/>
       <c r="C134"/>
       <c r="D134"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" s="7"/>
       <c r="C135"/>
       <c r="D135"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="7"/>
       <c r="C136"/>
       <c r="D136"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="7"/>
       <c r="C137"/>
       <c r="D137"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="7"/>
       <c r="C138"/>
       <c r="D138"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B139" s="7"/>
       <c r="C139"/>
       <c r="D139"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="7"/>
       <c r="C140"/>
       <c r="D140"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" s="7"/>
       <c r="C141"/>
       <c r="D141"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="7"/>
       <c r="C142"/>
       <c r="D142"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="7"/>
+      <c r="C143"/>
+      <c r="D143"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="7"/>
+      <c r="C144"/>
+      <c r="D144"/>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="7"/>
+      <c r="C145"/>
+      <c r="D145"/>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="7"/>
+      <c r="C146"/>
+      <c r="D146"/>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="7"/>
+      <c r="C147"/>
+      <c r="D147"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Extra text to locpar
</commit_message>
<xml_diff>
--- a/app/config/tables/PREGNANCIES/Forms/PREGNANCYFU/PREGNANCYFU.xlsx
+++ b/app/config/tables/PREGNANCIES/Forms/PREGNANCYFU/PREGNANCYFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0ADDDC-B9CF-49E7-8C70-A5DE099F8CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA449999-8040-4A47-93E5-50B0CB532236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="294">
   <si>
     <t>setting_name</t>
   </si>
@@ -921,6 +921,12 @@
   </si>
   <si>
     <t>Mulher ainda está no centro/hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At which health centre/clinic/hospital did the woman give birth? </t>
+  </si>
+  <si>
+    <t>Em que centro de saúde/clínica/hospital a mulher deu à luz?</t>
   </si>
 </sst>
 </file>
@@ -1467,11 +1473,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:T102"/>
+  <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2374,79 +2380,77 @@
       </c>
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>254</v>
-      </c>
-      <c r="E68" t="s">
-        <v>255</v>
-      </c>
-      <c r="F68" t="s">
-        <v>256</v>
+      <c r="D68" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="G68" s="17" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>266</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="S68" s="12"/>
     </row>
     <row r="69" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>254</v>
       </c>
       <c r="E69" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F69" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="G69" s="17" t="s">
-        <v>156</v>
+        <v>265</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="K69" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="T69" s="11" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
+        <v>254</v>
+      </c>
+      <c r="E70" t="s">
+        <v>257</v>
+      </c>
+      <c r="F70" t="s">
+        <v>263</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K70" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="T70" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
         <v>258</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>260</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F71" t="s">
         <v>264</v>
       </c>
-      <c r="S70" s="13" t="b">
+      <c r="S71" s="13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>67</v>
-      </c>
-      <c r="C71" t="s">
-        <v>278</v>
-      </c>
-      <c r="D71"/>
-      <c r="E71"/>
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>67</v>
       </c>
       <c r="C72" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D72"/>
       <c r="E72"/>
@@ -2456,171 +2460,180 @@
       <c r="I72"/>
     </row>
     <row r="73" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="D73" s="13" t="s">
+      <c r="B73" t="s">
+        <v>67</v>
+      </c>
+      <c r="C73" t="s">
+        <v>279</v>
+      </c>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
+      <c r="H73"/>
+      <c r="I73"/>
+    </row>
+    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F74" t="s">
         <v>259</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G74" t="s">
         <v>280</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H74" t="s">
         <v>281</v>
       </c>
-      <c r="K73" s="13" t="s">
+      <c r="K74" s="13" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>68</v>
       </c>
-      <c r="C74"/>
-      <c r="D74" s="13"/>
-      <c r="G74" s="13"/>
-    </row>
-    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C75"/>
-      <c r="D75" t="s">
+      <c r="D75" s="13"/>
+      <c r="G75" s="13"/>
+    </row>
+    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C76"/>
+      <c r="D76" t="s">
         <v>252</v>
       </c>
-      <c r="E75"/>
-      <c r="F75" t="s">
+      <c r="E76"/>
+      <c r="F76" t="s">
         <v>263</v>
       </c>
-      <c r="G75"/>
-      <c r="H75"/>
-      <c r="I75" t="s">
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76" t="s">
         <v>267</v>
       </c>
-      <c r="S75" s="13" t="b">
+      <c r="S76" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B77" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="78" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B78" s="13" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B79" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B80" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="13"/>
-    </row>
-    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D80" s="14" t="s">
+      <c r="D80" s="13"/>
+    </row>
+    <row r="81" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D81" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G80" s="17" t="s">
+      <c r="G81" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="H80" s="13" t="s">
+      <c r="H81" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="S80" s="12" t="b">
+      <c r="S81" s="12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
+    <row r="82" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
         <v>51</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E82" t="s">
         <v>53</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F82" t="s">
         <v>75</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G82" t="s">
         <v>102</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H82" t="s">
         <v>103</v>
       </c>
-      <c r="J81" s="13"/>
-      <c r="K81" t="s">
+      <c r="J82" s="13"/>
+      <c r="K82" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="82" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B82" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="83" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B83" s="13" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B84" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>163</v>
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B85" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B86" s="13" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="D86" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G86" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="H86" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="S86" s="12" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="87" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D87" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G87" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="S87" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D88" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E87" s="13" t="s">
+      <c r="E88" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G87" s="17" t="s">
+      <c r="G88" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="H87" s="13" t="s">
+      <c r="H88" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="L87" s="13" t="s">
+      <c r="L88" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="M87" s="13" t="s">
+      <c r="M88" s="13" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B88" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="89" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B89" s="13" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="2:19" x14ac:dyDescent="0.25">
@@ -2628,76 +2641,67 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>247</v>
+    <row r="91" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B91" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="92" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="93" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="93" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
-        <v>35</v>
-      </c>
-      <c r="G93" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="94" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
         <v>35</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H94" s="13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="95" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>35</v>
+      </c>
+      <c r="G95" t="s">
         <v>248</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H95" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="95" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
+    <row r="96" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B96" s="13" t="s">
+    <row r="97" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B97" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="97" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
+    <row r="98" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="98" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>35</v>
-      </c>
-      <c r="G98" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="S98" s="12" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
         <v>35</v>
       </c>
-      <c r="G99" t="s">
-        <v>113</v>
-      </c>
-      <c r="H99" t="s">
-        <v>114</v>
+      <c r="G99" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H99" s="13" t="s">
+        <v>212</v>
       </c>
       <c r="S99" s="12" t="b">
         <v>1</v>
@@ -2708,10 +2712,10 @@
         <v>35</v>
       </c>
       <c r="G100" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H100" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="S100" s="12" t="b">
         <v>1</v>
@@ -2719,20 +2723,34 @@
     </row>
     <row r="101" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
+        <v>35</v>
+      </c>
+      <c r="G101" t="s">
+        <v>115</v>
+      </c>
+      <c r="H101" t="s">
+        <v>116</v>
+      </c>
+      <c r="S101" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
         <v>60</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F102" t="s">
         <v>208</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G102" t="s">
         <v>209</v>
       </c>
-      <c r="H101" t="s">
+      <c r="H102" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="102" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
+    <row r="103" spans="2:19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2746,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>

</xml_diff>